<commit_message>
Renamed ins -> instr for instructions
</commit_message>
<xml_diff>
--- a/experiments_timeline.xlsx
+++ b/experiments_timeline.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UM MRes\UM projects\fNIRS_\stimulus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\github\breathwork-cognitive-psychopy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42751C31-CB1F-4AC9-B76A-919F079DE279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5360F7-0295-4A27-812D-C3159681D0C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="0" windowWidth="28695" windowHeight="15225" xr2:uid="{237ACA61-EE49-4979-BF8C-7A6B938B0AE0}"/>
+    <workbookView xWindow="60" yWindow="195" windowWidth="28695" windowHeight="15225" xr2:uid="{237ACA61-EE49-4979-BF8C-7A6B938B0AE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t>trigger code questions end</t>
   </si>
   <si>
-    <t>ins</t>
-  </si>
-  <si>
     <t>quit</t>
   </si>
   <si>
@@ -282,6 +279,9 @@
   </si>
   <si>
     <t>Example trigger sequence</t>
+  </si>
+  <si>
+    <t>instr</t>
   </si>
 </sst>
 </file>
@@ -716,7 +716,7 @@
   <dimension ref="A3:AX90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="AQ11" sqref="AQ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,7 +739,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -760,7 +760,7 @@
         <v>6</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="K3" s="1">
         <v>7</v>
@@ -772,7 +772,7 @@
         <v>9</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="O3" s="1">
         <v>10</v>
@@ -793,7 +793,7 @@
         <v>15</v>
       </c>
       <c r="U3" s="10" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="V3" s="1">
         <v>16</v>
@@ -805,7 +805,7 @@
         <v>18</v>
       </c>
       <c r="Y3" s="10" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="Z3" s="1">
         <v>19</v>
@@ -826,7 +826,7 @@
         <v>24</v>
       </c>
       <c r="AF3" s="10" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="AG3" s="4">
         <v>25</v>
@@ -838,7 +838,7 @@
         <v>27</v>
       </c>
       <c r="AJ3" s="10" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="AK3" s="4">
         <v>28</v>
@@ -859,7 +859,7 @@
         <v>33</v>
       </c>
       <c r="AQ3" s="10" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="AR3" s="1">
         <v>34</v>
@@ -880,7 +880,7 @@
         <v>39</v>
       </c>
       <c r="AX3" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.25">
@@ -1068,7 +1068,7 @@
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1238,367 +1238,367 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>